<commit_message>
adding readme and fixed no isotope input
</commit_message>
<xml_diff>
--- a/InteractiveMean/stats/Stats_mapa1quant.xlsx
+++ b/InteractiveMean/stats/Stats_mapa1quant.xlsx
@@ -526,336 +526,30 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>932.9116645301752</v>
-      </c>
-      <c r="C2">
-        <v>778.8013939023356</v>
-      </c>
-      <c r="D2">
-        <v>189910.56379896</v>
-      </c>
-      <c r="E2">
-        <v>4718.373706132841</v>
-      </c>
-      <c r="F2">
-        <v>378105.9665546579</v>
-      </c>
-      <c r="G2">
-        <v>145.4561817507357</v>
-      </c>
-      <c r="H2">
-        <v>3587.057357193459</v>
-      </c>
-      <c r="I2">
-        <v>7.868434396734703</v>
-      </c>
-      <c r="J2">
-        <v>275.6954782730438</v>
-      </c>
-      <c r="K2">
-        <v>690.648582134508</v>
-      </c>
-      <c r="L2">
-        <v>93.88315413995399</v>
-      </c>
-      <c r="M2">
-        <v>406.4305098895159</v>
-      </c>
-      <c r="N2">
-        <v>16.84975424660496</v>
-      </c>
-      <c r="O2">
-        <v>41.5853632438418</v>
-      </c>
-      <c r="P2">
-        <v>15.34214875289505</v>
-      </c>
-      <c r="Q2">
-        <v>2.223609260884532</v>
-      </c>
-      <c r="R2">
-        <v>4.436122003297145</v>
-      </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>325.9796315942217</v>
-      </c>
-      <c r="C3">
-        <v>1895.288559226827</v>
-      </c>
-      <c r="D3">
-        <v>53870.74906998981</v>
-      </c>
-      <c r="E3">
-        <v>6601.18196548169</v>
-      </c>
-      <c r="F3">
-        <v>97231.54269291609</v>
-      </c>
-      <c r="G3">
-        <v>287.7507797618063</v>
-      </c>
-      <c r="H3">
-        <v>772.324984101654</v>
-      </c>
-      <c r="I3">
-        <v>13.5079020991301</v>
-      </c>
-      <c r="J3">
-        <v>80.97836439574493</v>
-      </c>
-      <c r="K3">
-        <v>201.6158528076056</v>
-      </c>
-      <c r="L3">
-        <v>27.127016576435</v>
-      </c>
-      <c r="M3">
-        <v>119.0440575035294</v>
-      </c>
-      <c r="N3">
-        <v>4.968107612579697</v>
-      </c>
-      <c r="O3">
-        <v>12.78270121479772</v>
-      </c>
-      <c r="P3">
-        <v>4.887752290515908</v>
-      </c>
-      <c r="Q3">
-        <v>0.7548220574342314</v>
-      </c>
-      <c r="R3">
-        <v>1.614905806665006</v>
-      </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>125010.1630470435</v>
-      </c>
-      <c r="C4">
-        <v>104359.386782913</v>
-      </c>
-      <c r="D4">
-        <v>25448015.54906064</v>
-      </c>
-      <c r="E4">
-        <v>632262.0766218007</v>
-      </c>
-      <c r="F4">
-        <v>50666199.51832416</v>
-      </c>
-      <c r="G4">
-        <v>19491.12835459859</v>
-      </c>
-      <c r="H4">
-        <v>480665.6858639235</v>
-      </c>
-      <c r="I4">
-        <v>1054.37020916245</v>
-      </c>
-      <c r="J4">
-        <v>36943.19408858787</v>
-      </c>
-      <c r="K4">
-        <v>92546.91000602407</v>
-      </c>
-      <c r="L4">
-        <v>12580.34265475383</v>
-      </c>
-      <c r="M4">
-        <v>54461.68832519512</v>
-      </c>
-      <c r="N4">
-        <v>2257.867069045064</v>
-      </c>
-      <c r="O4">
-        <v>5572.438674674801</v>
-      </c>
-      <c r="P4">
-        <v>2055.847932887937</v>
-      </c>
-      <c r="Q4">
-        <v>297.9636409585273</v>
-      </c>
-      <c r="R4">
-        <v>594.4403484418174</v>
-      </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>12.00227289869241</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1101.233455242116</v>
-      </c>
-      <c r="G5">
-        <v>3.64712853400721</v>
-      </c>
-      <c r="H5">
-        <v>2.568606088759509</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>2462.862569421069</v>
-      </c>
-      <c r="C6">
-        <v>14686.95196935894</v>
-      </c>
-      <c r="D6">
-        <v>244369.803222501</v>
-      </c>
-      <c r="E6">
-        <v>35223.0003309797</v>
-      </c>
-      <c r="F6">
-        <v>961833.9366131532</v>
-      </c>
-      <c r="G6">
-        <v>2536.332543118818</v>
-      </c>
-      <c r="H6">
-        <v>7641.981555356615</v>
-      </c>
-      <c r="I6">
-        <v>151.4743183763863</v>
-      </c>
-      <c r="J6">
-        <v>389.4905302467069</v>
-      </c>
-      <c r="K6">
-        <v>1013.888842909696</v>
-      </c>
-      <c r="L6">
-        <v>129.562163786305</v>
-      </c>
-      <c r="M6">
-        <v>579.1330416797442</v>
-      </c>
-      <c r="N6">
-        <v>27.07650356847699</v>
-      </c>
-      <c r="O6">
-        <v>65.1527448975297</v>
-      </c>
-      <c r="P6">
-        <v>23.54648341603226</v>
-      </c>
-      <c r="Q6">
-        <v>3.979652553101639</v>
-      </c>
-      <c r="R6">
-        <v>9.309087337055974</v>
-      </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>6</v>
-      </c>
-      <c r="B7">
-        <v>959.5347191972151</v>
-      </c>
-      <c r="C7">
-        <v>210.9786201849704</v>
-      </c>
-      <c r="D7">
-        <v>206386.890563666</v>
-      </c>
-      <c r="E7">
-        <v>1767.297137025596</v>
-      </c>
-      <c r="F7">
-        <v>366194.2489934226</v>
-      </c>
-      <c r="G7">
-        <v>64.89125814370706</v>
-      </c>
-      <c r="H7">
-        <v>3696.6527859743</v>
-      </c>
-      <c r="I7">
-        <v>6.731743144963062</v>
-      </c>
-      <c r="J7">
-        <v>289.4971313062566</v>
-      </c>
-      <c r="K7">
-        <v>731.0172264793421</v>
-      </c>
-      <c r="L7">
-        <v>98.82422352170829</v>
-      </c>
-      <c r="M7">
-        <v>426.5095726601767</v>
-      </c>
-      <c r="N7">
-        <v>17.74393863198977</v>
-      </c>
-      <c r="O7">
-        <v>44.09618495582823</v>
-      </c>
-      <c r="P7">
-        <v>15.95901286469767</v>
-      </c>
-      <c r="Q7">
-        <v>2.283369770307985</v>
-      </c>
-      <c r="R7">
-        <v>4.559459931212493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>